<commit_message>
Added try catch block to all the developed methods
</commit_message>
<xml_diff>
--- a/AutomatedTest/TestData/Temenos/ManualReject.xlsx
+++ b/AutomatedTest/TestData/Temenos/ManualReject.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC33A537-8A52-42AC-9926-53070A82CBA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1180DF96-AAE5-4BBC-A94E-DEB52094D1D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="InputTestData" sheetId="2" r:id="rId2"/>
     <sheet name="ValidationTestData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -104,9 +104,6 @@
     <t>AccountNumber</t>
   </si>
   <si>
-    <t>Applicationtype</t>
-  </si>
-  <si>
     <t>ApproveApplyingFor</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Term</t>
+  </si>
+  <si>
+    <t>ApplicationType</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,16 +898,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>29</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>24</v>
@@ -916,16 +916,16 @@
         <v>25</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>16</v>
@@ -965,19 +965,19 @@
     </row>
     <row r="3" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>8</v>

</xml_diff>